<commit_message>
commit para borrar carpeta target
</commit_message>
<xml_diff>
--- a/target/test-classes/test.xlsx
+++ b/target/test-classes/test.xlsx
@@ -1,36 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27907"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/herminio/Git/citizens0/src/test/resources/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="25600" windowHeight="15480"/>
+    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Nombre</t>
   </si>
@@ -38,51 +22,6 @@
     <t>90500084Y</t>
   </si>
   <si>
-    <t>19160962F</t>
-  </si>
-  <si>
-    <t>09940449X</t>
-  </si>
-  <si>
-    <t>C/ Federico García Lorca 2</t>
-  </si>
-  <si>
-    <t>C/ Real Oviedo 2</t>
-  </si>
-  <si>
-    <t>Av. De la Constitución 8</t>
-  </si>
-  <si>
-    <t>Apellidos</t>
-  </si>
-  <si>
-    <t>Juan</t>
-  </si>
-  <si>
-    <t>Torres Pardo</t>
-  </si>
-  <si>
-    <t>Luis</t>
-  </si>
-  <si>
-    <t>López Fernando</t>
-  </si>
-  <si>
-    <t>Ana</t>
-  </si>
-  <si>
-    <t>DNI</t>
-  </si>
-  <si>
-    <t>Fecha nacimiento</t>
-  </si>
-  <si>
-    <t>Nacionalidad</t>
-  </si>
-  <si>
-    <t>Español</t>
-  </si>
-  <si>
     <t>Correo electrónico</t>
   </si>
   <si>
@@ -92,10 +31,37 @@
     <t>luis@example.com</t>
   </si>
   <si>
-    <t>ana@example.com</t>
-  </si>
-  <si>
-    <t>Dirección postal</t>
+    <t>Localización</t>
+  </si>
+  <si>
+    <t>Identificador</t>
+  </si>
+  <si>
+    <t>Tipo</t>
+  </si>
+  <si>
+    <t>Juan Torres Pardo</t>
+  </si>
+  <si>
+    <t>Sensor temperatura S1</t>
+  </si>
+  <si>
+    <t>ST1Oviedo</t>
+  </si>
+  <si>
+    <t>Universidad de Oviedo</t>
+  </si>
+  <si>
+    <t>uniovi@example.com</t>
+  </si>
+  <si>
+    <t>Q3318001I</t>
+  </si>
+  <si>
+    <t>43.36;-5.85</t>
+  </si>
+  <si>
+    <t>43.24;-5.78</t>
   </si>
 </sst>
 </file>
@@ -143,8 +109,8 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -156,9 +122,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -419,7 +382,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -430,113 +393,90 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="22.1640625" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.42578125" customWidth="1"/>
+    <col min="4" max="4" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2"/>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="C4" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="2">
-        <v>31330</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="2">
-        <v>25629</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="E4" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" s="3">
-        <v>21916</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="C3" r:id="rId2"/>
-    <hyperlink ref="C4" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>

</xml_diff>